<commit_message>
Hybrid Framework Project Last commit
</commit_message>
<xml_diff>
--- a/target/test-classes/testdata/excels/regression/Adactin Master Test Data.xlsx
+++ b/target/test-classes/testdata/excels/regression/Adactin Master Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\006LiveTechWS\HybridFramework\src\test\resources\testdata\excels\regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B3A08C-C79C-4A3E-95C0-3B02F037A168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98777DC-DCA8-413D-8D5C-2223CF492667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ECA7341F-7CE3-4EA7-B2BF-C9C26B540FCF}"/>
   </bookViews>
@@ -557,7 +557,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>

</xml_diff>